<commit_message>
Toimii nyt myös US aikaleimoilla
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trelehtija\Desktop\Master\Omat projektit\generate_xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3989857-50AD-4B17-BD48-74B4DC455662}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC16D9BE-B48C-4AF0-8E8F-E1ED43D07194}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,13 +117,13 @@
     <t>Hour</t>
   </si>
   <si>
-    <t>Week</t>
-  </si>
-  <si>
     <t>timeFormat</t>
   </si>
   <si>
     <t>US</t>
+  </si>
+  <si>
+    <t>Month</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +493,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -513,13 +513,13 @@
         <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
         <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -539,7 +539,7 @@
         <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>
@@ -562,7 +562,7 @@
         <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
@@ -585,7 +585,7 @@
         <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
@@ -608,7 +608,7 @@
         <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
@@ -631,7 +631,7 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
         <v>27</v>
@@ -654,7 +654,7 @@
         <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
         <v>27</v>
@@ -677,7 +677,7 @@
         <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
         <v>27</v>
@@ -700,7 +700,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G10" t="s">
         <v>27</v>
@@ -723,7 +723,7 @@
         <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G11" t="s">
         <v>27</v>
@@ -746,7 +746,7 @@
         <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s">
         <v>27</v>
@@ -769,7 +769,7 @@
         <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G13" t="s">
         <v>27</v>
@@ -792,7 +792,7 @@
         <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
         <v>27</v>
@@ -815,7 +815,7 @@
         <v>24</v>
       </c>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G15" t="s">
         <v>27</v>
@@ -838,7 +838,7 @@
         <v>24</v>
       </c>
       <c r="F16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s">
         <v>27</v>
@@ -861,7 +861,7 @@
         <v>24</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G17" t="s">
         <v>27</v>
@@ -884,7 +884,7 @@
         <v>24</v>
       </c>
       <c r="F18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G18" t="s">
         <v>27</v>

</xml_diff>